<commit_message>
Migrate Excel creation to XSSF backend
To be able to operate with Excel templates
containing diagrams, the backend for Excel
generation is migrated to the XSSF one.
This required major refactorings in
`ExcelGenerator` and `ExcelWriter`.
The creation workflow is now similar to the
Word generation, as the template is modified,
loops inserted after the placeholder block, and
removing the block after finishing its
generation.
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/excel/CollectionsTemplate.xlsx
+++ b/src/test/resources/templates/excel/CollectionsTemplate.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -167,19 +167,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,15 +255,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,10 +453,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Migrate Excel creation to XSSF backend (#254)
To be able to operate with Excel templates
containing diagrams, the backend for Excel
generation is migrated to the XSSF one.
This required major refactorings in
`ExcelGenerator` and `ExcelWriter`.
The creation workflow is now similar to the
Word generation, as the template is modified,
loops inserted after the placeholder block, and
removing the block after finishing its
generation.
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/excel/CollectionsTemplate.xlsx
+++ b/src/test/resources/templates/excel/CollectionsTemplate.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -167,19 +167,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,15 +255,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,10 +453,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>